<commit_message>
added functions for AOCS sizing
</commit_message>
<xml_diff>
--- a/organizational/iterations_io.xlsx
+++ b/organizational/iterations_io.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12420" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12420" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="123">
   <si>
     <t>Pointing Direction</t>
   </si>
@@ -417,6 +417,15 @@
   </si>
   <si>
     <t>Probes</t>
+  </si>
+  <si>
+    <t>Nominal rates</t>
+  </si>
+  <si>
+    <t>Full range</t>
+  </si>
+  <si>
+    <t>Nominal (0.05 - 0.5 deg/s)</t>
   </si>
 </sst>
 </file>
@@ -914,7 +923,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1186,6 +1195,15 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1204,54 +1222,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Explanatory Text" xfId="3" builtinId="53"/>
@@ -1882,7 +1893,7 @@
   <dimension ref="A1:I71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1892,7 +1903,7 @@
     <col min="4" max="4" width="19.5703125" style="19" customWidth="1"/>
     <col min="5" max="5" width="20.7109375" style="4" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" style="42" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" style="42" customWidth="1"/>
+    <col min="7" max="7" width="24" style="42" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="42.5703125" style="4" customWidth="1"/>
   </cols>
@@ -1906,27 +1917,27 @@
       <c r="A2" s="96" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="119" t="s">
+      <c r="D2" s="111" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="120"/>
-      <c r="F2" s="120"/>
-      <c r="G2" s="120"/>
-      <c r="H2" s="120"/>
-      <c r="I2" s="121"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
+      <c r="H2" s="112"/>
+      <c r="I2" s="113"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="97" t="s">
         <v>56</v>
       </c>
-      <c r="D3" s="128" t="s">
+      <c r="D3" s="126" t="s">
         <v>61</v>
       </c>
-      <c r="E3" s="129"/>
-      <c r="F3" s="128" t="s">
+      <c r="E3" s="127"/>
+      <c r="F3" s="126" t="s">
         <v>62</v>
       </c>
-      <c r="G3" s="130"/>
+      <c r="G3" s="128"/>
       <c r="H3" s="66"/>
       <c r="I3" s="88"/>
     </row>
@@ -1954,7 +1965,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="117" t="s">
+      <c r="C5" s="129" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="49" t="s">
@@ -1963,10 +1974,10 @@
       <c r="E5" s="60" t="s">
         <v>52</v>
       </c>
-      <c r="F5" s="118" t="s">
+      <c r="F5" s="130" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="122" t="s">
+      <c r="G5" s="120" t="s">
         <v>73</v>
       </c>
       <c r="H5" s="50"/>
@@ -1975,59 +1986,59 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C6" s="112"/>
+      <c r="C6" s="115"/>
       <c r="D6" s="43" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="F6" s="115"/>
-      <c r="G6" s="123"/>
+      <c r="F6" s="118"/>
+      <c r="G6" s="121"/>
       <c r="H6" s="44"/>
       <c r="I6" s="36"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C7" s="112"/>
+      <c r="C7" s="115"/>
       <c r="D7" s="43" t="s">
         <v>47</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="F7" s="115"/>
-      <c r="G7" s="123"/>
+      <c r="F7" s="118"/>
+      <c r="G7" s="121"/>
       <c r="H7" s="44"/>
       <c r="I7" s="36"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C8" s="112"/>
+      <c r="C8" s="115"/>
       <c r="D8" s="43" t="s">
         <v>5</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="F8" s="115"/>
-      <c r="G8" s="123"/>
+      <c r="F8" s="118"/>
+      <c r="G8" s="121"/>
       <c r="H8" s="44"/>
       <c r="I8" s="36"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C9" s="113"/>
+      <c r="C9" s="116"/>
       <c r="D9" s="43" t="s">
         <v>50</v>
       </c>
       <c r="E9" s="71" t="s">
         <v>54</v>
       </c>
-      <c r="F9" s="116"/>
-      <c r="G9" s="124"/>
+      <c r="F9" s="119"/>
+      <c r="G9" s="122"/>
       <c r="H9" s="44"/>
       <c r="I9" s="36"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C10" s="125" t="s">
+      <c r="C10" s="123" t="s">
         <v>48</v>
       </c>
       <c r="D10" s="54" t="s">
@@ -2050,7 +2061,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C11" s="126"/>
+      <c r="C11" s="124"/>
       <c r="D11" s="43" t="s">
         <v>7</v>
       </c>
@@ -2065,7 +2076,7 @@
       <c r="I11" s="36"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="127"/>
+      <c r="C12" s="125"/>
       <c r="D12" s="57" t="s">
         <v>50</v>
       </c>
@@ -2078,7 +2089,7 @@
       <c r="I12" s="92"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C13" s="111" t="s">
+      <c r="C13" s="114" t="s">
         <v>49</v>
       </c>
       <c r="D13" s="43" t="s">
@@ -2090,14 +2101,14 @@
       <c r="F13" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="G13" s="83" t="s">
-        <v>90</v>
+      <c r="G13" t="s">
+        <v>121</v>
       </c>
       <c r="H13" s="44"/>
       <c r="I13" s="36"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C14" s="112"/>
+      <c r="C14" s="115"/>
       <c r="D14" s="43" t="s">
         <v>7</v>
       </c>
@@ -2116,12 +2127,12 @@
       <c r="I14" s="36"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C15" s="112"/>
+      <c r="C15" s="115"/>
       <c r="D15" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="E15" s="81" t="s">
-        <v>90</v>
+      <c r="E15" t="s">
+        <v>120</v>
       </c>
       <c r="F15" s="52" t="s">
         <v>69</v>
@@ -2133,7 +2144,7 @@
       <c r="I15" s="36"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C16" s="113"/>
+      <c r="C16" s="116"/>
       <c r="D16" s="57" t="s">
         <v>110</v>
       </c>
@@ -2143,14 +2154,14 @@
       <c r="F16" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="G16" s="85" t="s">
-        <v>90</v>
+      <c r="G16" s="58" t="s">
+        <v>122</v>
       </c>
       <c r="H16" s="58"/>
       <c r="I16" s="92"/>
     </row>
     <row r="17" spans="3:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="C17" s="111" t="s">
+      <c r="C17" s="114" t="s">
         <v>75</v>
       </c>
       <c r="D17" s="43" t="s">
@@ -2164,7 +2175,7 @@
 Slew
 Safe</v>
       </c>
-      <c r="F17" s="114" t="s">
+      <c r="F17" s="117" t="s">
         <v>79</v>
       </c>
       <c r="G17" s="75"/>
@@ -2174,14 +2185,14 @@
       </c>
     </row>
     <row r="18" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C18" s="112"/>
+      <c r="C18" s="115"/>
       <c r="D18" s="43" t="s">
         <v>91</v>
       </c>
       <c r="E18" s="94" t="s">
         <v>90</v>
       </c>
-      <c r="F18" s="115"/>
+      <c r="F18" s="118"/>
       <c r="G18" s="75" t="s">
         <v>80</v>
       </c>
@@ -2189,18 +2200,18 @@
       <c r="I18" s="36"/>
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C19" s="112"/>
+      <c r="C19" s="115"/>
       <c r="D19" s="43" t="s">
         <v>71</v>
       </c>
       <c r="E19" s="9"/>
-      <c r="F19" s="115"/>
+      <c r="F19" s="118"/>
       <c r="G19" s="75"/>
       <c r="H19" s="44"/>
       <c r="I19" s="36"/>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C20" s="112"/>
+      <c r="C20" s="115"/>
       <c r="D20" s="43" t="s">
         <v>63</v>
       </c>
@@ -2208,33 +2219,33 @@
         <f>G10</f>
         <v>0.1 - 0.5 deg</v>
       </c>
-      <c r="F20" s="115"/>
+      <c r="F20" s="118"/>
       <c r="G20" s="75"/>
       <c r="H20" s="44"/>
       <c r="I20" s="36"/>
     </row>
     <row r="21" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C21" s="113"/>
+      <c r="C21" s="116"/>
       <c r="D21" s="57" t="s">
         <v>77</v>
       </c>
       <c r="E21" s="93" t="s">
         <v>78</v>
       </c>
-      <c r="F21" s="116"/>
+      <c r="F21" s="119"/>
       <c r="G21" s="74"/>
       <c r="H21" s="58"/>
       <c r="I21" s="92"/>
     </row>
     <row r="22" spans="3:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="C22" s="111" t="s">
+      <c r="C22" s="114" t="s">
         <v>82</v>
       </c>
       <c r="D22" s="54" t="s">
         <v>96</v>
       </c>
       <c r="E22" s="6"/>
-      <c r="F22" s="114" t="s">
+      <c r="F22" s="117" t="s">
         <v>98</v>
       </c>
       <c r="G22" s="73"/>
@@ -2242,36 +2253,36 @@
       <c r="I22" s="56"/>
     </row>
     <row r="23" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C23" s="112"/>
+      <c r="C23" s="115"/>
       <c r="D23" s="43" t="s">
         <v>99</v>
       </c>
       <c r="E23" s="9"/>
-      <c r="F23" s="115"/>
+      <c r="F23" s="118"/>
       <c r="G23" s="75"/>
       <c r="H23" s="44"/>
       <c r="I23" s="45"/>
     </row>
     <row r="24" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C24" s="113"/>
+      <c r="C24" s="116"/>
       <c r="D24" s="57" t="s">
         <v>97</v>
       </c>
       <c r="E24" s="99"/>
-      <c r="F24" s="116"/>
+      <c r="F24" s="119"/>
       <c r="G24" s="74"/>
       <c r="H24" s="58"/>
       <c r="I24" s="59"/>
     </row>
     <row r="25" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C25" s="111" t="s">
+      <c r="C25" s="114" t="s">
         <v>100</v>
       </c>
       <c r="D25" s="54" t="s">
         <v>101</v>
       </c>
       <c r="E25" s="6"/>
-      <c r="F25" s="114" t="s">
+      <c r="F25" s="117" t="s">
         <v>105</v>
       </c>
       <c r="G25" s="73"/>
@@ -2279,23 +2290,23 @@
       <c r="I25" s="91"/>
     </row>
     <row r="26" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C26" s="112"/>
+      <c r="C26" s="115"/>
       <c r="D26" s="43" t="s">
         <v>63</v>
       </c>
       <c r="E26" s="9"/>
-      <c r="F26" s="115"/>
+      <c r="F26" s="118"/>
       <c r="G26" s="75"/>
       <c r="H26" s="44"/>
       <c r="I26" s="36"/>
     </row>
     <row r="27" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C27" s="112"/>
+      <c r="C27" s="115"/>
       <c r="D27" s="43" t="s">
         <v>102</v>
       </c>
       <c r="E27" s="9"/>
-      <c r="F27" s="115" t="s">
+      <c r="F27" s="118" t="s">
         <v>106</v>
       </c>
       <c r="G27" s="75"/>
@@ -2303,23 +2314,23 @@
       <c r="I27" s="36"/>
     </row>
     <row r="28" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C28" s="112"/>
+      <c r="C28" s="115"/>
       <c r="D28" s="43" t="s">
         <v>49</v>
       </c>
       <c r="E28" s="9"/>
-      <c r="F28" s="115"/>
+      <c r="F28" s="118"/>
       <c r="G28" s="75"/>
       <c r="H28" s="44"/>
       <c r="I28" s="36"/>
     </row>
     <row r="29" spans="3:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="C29" s="112"/>
+      <c r="C29" s="115"/>
       <c r="D29" s="43" t="s">
         <v>103</v>
       </c>
       <c r="E29" s="9"/>
-      <c r="F29" s="115" t="s">
+      <c r="F29" s="118" t="s">
         <v>107</v>
       </c>
       <c r="G29" s="75"/>
@@ -2327,12 +2338,12 @@
       <c r="I29" s="36"/>
     </row>
     <row r="30" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C30" s="113"/>
+      <c r="C30" s="116"/>
       <c r="D30" s="57" t="s">
         <v>104</v>
       </c>
       <c r="E30" s="11"/>
-      <c r="F30" s="116"/>
+      <c r="F30" s="119"/>
       <c r="G30" s="74"/>
       <c r="H30" s="58"/>
       <c r="I30" s="92"/>
@@ -2710,6 +2721,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C25:C30"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="C5:C9"/>
+    <mergeCell ref="F5:F9"/>
     <mergeCell ref="D2:I2"/>
     <mergeCell ref="C17:C21"/>
     <mergeCell ref="C13:C16"/>
@@ -2720,12 +2737,6 @@
     <mergeCell ref="C10:C12"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:G3"/>
-    <mergeCell ref="C25:C30"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="C5:C9"/>
-    <mergeCell ref="F5:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2735,8 +2746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2756,27 +2767,27 @@
       <c r="A2" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="119" t="s">
+      <c r="D2" s="111" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="120"/>
-      <c r="F2" s="120"/>
-      <c r="G2" s="120"/>
-      <c r="H2" s="120"/>
-      <c r="I2" s="121"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
+      <c r="H2" s="112"/>
+      <c r="I2" s="113"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="69" t="s">
         <v>56</v>
       </c>
-      <c r="D3" s="128" t="s">
+      <c r="D3" s="126" t="s">
         <v>61</v>
       </c>
-      <c r="E3" s="129"/>
-      <c r="F3" s="128" t="s">
+      <c r="E3" s="127"/>
+      <c r="F3" s="126" t="s">
         <v>62</v>
       </c>
-      <c r="G3" s="130"/>
+      <c r="G3" s="128"/>
       <c r="H3" s="66"/>
       <c r="I3" s="67"/>
     </row>
@@ -2804,7 +2815,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C5" s="117" t="s">
+      <c r="C5" s="129" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="49" t="s">
@@ -2816,7 +2827,7 @@
       <c r="F5" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="122" t="s">
+      <c r="G5" s="120" t="s">
         <v>83</v>
       </c>
       <c r="H5" s="50"/>
@@ -2825,7 +2836,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C6" s="112"/>
+      <c r="C6" s="115"/>
       <c r="D6" s="43" t="s">
         <v>7</v>
       </c>
@@ -2833,14 +2844,14 @@
         <v>31</v>
       </c>
       <c r="F6" s="52"/>
-      <c r="G6" s="123"/>
+      <c r="G6" s="121"/>
       <c r="H6" s="44" t="s">
         <v>75</v>
       </c>
       <c r="I6" s="45"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C7" s="112"/>
+      <c r="C7" s="115"/>
       <c r="D7" s="43" t="s">
         <v>6</v>
       </c>
@@ -2848,12 +2859,12 @@
         <v>32</v>
       </c>
       <c r="F7" s="52"/>
-      <c r="G7" s="123"/>
+      <c r="G7" s="121"/>
       <c r="H7" s="44"/>
       <c r="I7" s="45"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C8" s="113"/>
+      <c r="C8" s="116"/>
       <c r="D8" s="43" t="s">
         <v>50</v>
       </c>
@@ -2861,12 +2872,12 @@
         <v>34</v>
       </c>
       <c r="F8" s="102"/>
-      <c r="G8" s="124"/>
+      <c r="G8" s="122"/>
       <c r="H8" s="44"/>
       <c r="I8" s="45"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C9" s="125" t="s">
+      <c r="C9" s="123" t="s">
         <v>48</v>
       </c>
       <c r="D9" s="54" t="s">
@@ -2885,7 +2896,7 @@
       <c r="I9" s="56"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C10" s="126"/>
+      <c r="C10" s="124"/>
       <c r="D10" s="43" t="s">
         <v>7</v>
       </c>
@@ -2902,7 +2913,7 @@
       <c r="I10" s="45"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C11" s="127"/>
+      <c r="C11" s="125"/>
       <c r="D11" s="57" t="s">
         <v>6</v>
       </c>
@@ -2915,7 +2926,7 @@
       <c r="I11" s="59"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="111" t="s">
+      <c r="C12" s="114" t="s">
         <v>49</v>
       </c>
       <c r="D12" s="43" t="s">
@@ -2934,7 +2945,7 @@
       <c r="I12" s="45"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C13" s="112"/>
+      <c r="C13" s="115"/>
       <c r="D13" s="43"/>
       <c r="E13" s="9"/>
       <c r="F13" s="52" t="s">
@@ -2949,7 +2960,7 @@
       <c r="I13" s="45"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C14" s="112"/>
+      <c r="C14" s="115"/>
       <c r="D14" s="43" t="s">
         <v>7</v>
       </c>
@@ -2966,7 +2977,7 @@
       <c r="I14" s="45"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C15" s="113"/>
+      <c r="C15" s="116"/>
       <c r="D15" s="57" t="s">
         <v>47</v>
       </c>
@@ -2983,7 +2994,7 @@
       <c r="I15" s="59"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C16" s="111" t="s">
+      <c r="C16" s="114" t="s">
         <v>75</v>
       </c>
       <c r="D16" s="43" t="s">
@@ -2992,7 +3003,7 @@
       <c r="E16" t="s">
         <v>81</v>
       </c>
-      <c r="F16" s="114" t="s">
+      <c r="F16" s="117" t="s">
         <v>79</v>
       </c>
       <c r="G16" s="75"/>
@@ -3002,14 +3013,14 @@
       </c>
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C17" s="112"/>
+      <c r="C17" s="115"/>
       <c r="D17" s="43" t="s">
         <v>76</v>
       </c>
       <c r="E17" s="77" t="s">
         <v>81</v>
       </c>
-      <c r="F17" s="115"/>
+      <c r="F17" s="118"/>
       <c r="G17" s="75" t="s">
         <v>80</v>
       </c>
@@ -3017,14 +3028,14 @@
       <c r="I17" s="132"/>
     </row>
     <row r="18" spans="3:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="C18" s="112"/>
+      <c r="C18" s="115"/>
       <c r="D18" s="43" t="s">
         <v>87</v>
       </c>
       <c r="E18" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="115"/>
+      <c r="F18" s="118"/>
       <c r="G18" s="75"/>
       <c r="H18" s="44"/>
       <c r="I18" s="28" t="s">
@@ -3032,7 +3043,7 @@
       </c>
     </row>
     <row r="19" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C19" s="112"/>
+      <c r="C19" s="115"/>
       <c r="D19" s="43" t="s">
         <v>89</v>
       </c>
@@ -3040,33 +3051,33 @@
         <f>G9</f>
         <v>not used</v>
       </c>
-      <c r="F19" s="115"/>
+      <c r="F19" s="118"/>
       <c r="G19" s="75"/>
       <c r="H19" s="44"/>
       <c r="I19" s="28"/>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C20" s="113"/>
+      <c r="C20" s="116"/>
       <c r="D20" s="57" t="s">
         <v>77</v>
       </c>
       <c r="E20" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="F20" s="116"/>
+      <c r="F20" s="119"/>
       <c r="G20" s="74"/>
       <c r="H20" s="58"/>
       <c r="I20" s="79"/>
     </row>
     <row r="21" spans="3:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="111" t="s">
+      <c r="C21" s="114" t="s">
         <v>82</v>
       </c>
       <c r="D21" s="54" t="s">
         <v>96</v>
       </c>
       <c r="E21" s="6"/>
-      <c r="F21" s="114" t="s">
+      <c r="F21" s="117" t="s">
         <v>98</v>
       </c>
       <c r="G21" s="73"/>
@@ -3074,36 +3085,36 @@
       <c r="I21" s="56"/>
     </row>
     <row r="22" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C22" s="112"/>
+      <c r="C22" s="115"/>
       <c r="D22" s="43" t="s">
         <v>95</v>
       </c>
       <c r="E22" s="9"/>
-      <c r="F22" s="115"/>
+      <c r="F22" s="118"/>
       <c r="G22" s="75"/>
       <c r="H22" s="44"/>
       <c r="I22" s="45"/>
     </row>
     <row r="23" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C23" s="113"/>
+      <c r="C23" s="116"/>
       <c r="D23" s="57" t="s">
         <v>97</v>
       </c>
       <c r="E23" s="99"/>
-      <c r="F23" s="116"/>
+      <c r="F23" s="119"/>
       <c r="G23" s="74"/>
       <c r="H23" s="58"/>
       <c r="I23" s="59"/>
     </row>
     <row r="24" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C24" s="111" t="s">
+      <c r="C24" s="114" t="s">
         <v>100</v>
       </c>
       <c r="D24" s="54" t="s">
         <v>101</v>
       </c>
       <c r="E24" s="6"/>
-      <c r="F24" s="114" t="s">
+      <c r="F24" s="117" t="s">
         <v>105</v>
       </c>
       <c r="G24" s="73"/>
@@ -3111,23 +3122,23 @@
       <c r="I24" s="91"/>
     </row>
     <row r="25" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C25" s="112"/>
+      <c r="C25" s="115"/>
       <c r="D25" s="43" t="s">
         <v>63</v>
       </c>
       <c r="E25" s="9"/>
-      <c r="F25" s="115"/>
+      <c r="F25" s="118"/>
       <c r="G25" s="75"/>
       <c r="H25" s="44"/>
       <c r="I25" s="36"/>
     </row>
     <row r="26" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C26" s="112"/>
+      <c r="C26" s="115"/>
       <c r="D26" s="43" t="s">
         <v>102</v>
       </c>
       <c r="E26" s="9"/>
-      <c r="F26" s="115" t="s">
+      <c r="F26" s="118" t="s">
         <v>106</v>
       </c>
       <c r="G26" s="75"/>
@@ -3135,23 +3146,23 @@
       <c r="I26" s="36"/>
     </row>
     <row r="27" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C27" s="112"/>
+      <c r="C27" s="115"/>
       <c r="D27" s="43" t="s">
         <v>49</v>
       </c>
       <c r="E27" s="9"/>
-      <c r="F27" s="115"/>
+      <c r="F27" s="118"/>
       <c r="G27" s="75"/>
       <c r="H27" s="44"/>
       <c r="I27" s="36"/>
     </row>
     <row r="28" spans="3:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="C28" s="112"/>
+      <c r="C28" s="115"/>
       <c r="D28" s="43" t="s">
         <v>103</v>
       </c>
       <c r="E28" s="9"/>
-      <c r="F28" s="115" t="s">
+      <c r="F28" s="118" t="s">
         <v>107</v>
       </c>
       <c r="G28" s="75"/>
@@ -3159,12 +3170,12 @@
       <c r="I28" s="36"/>
     </row>
     <row r="29" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C29" s="113"/>
+      <c r="C29" s="116"/>
       <c r="D29" s="57" t="s">
         <v>104</v>
       </c>
       <c r="E29" s="11"/>
-      <c r="F29" s="116"/>
+      <c r="F29" s="119"/>
       <c r="G29" s="74"/>
       <c r="H29" s="58"/>
       <c r="I29" s="92"/>
@@ -3542,22 +3553,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="F16:F20"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="C16:C20"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="C24:C29"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="F21:F23"/>
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="D2:I2"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="C5:C8"/>
     <mergeCell ref="G5:G8"/>
-    <mergeCell ref="C24:C29"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="F16:F20"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="C16:C20"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="I16:I17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3568,84 +3579,102 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:A16"/>
+  <dimension ref="A2:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="134" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="133" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" s="134">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B7" s="134">
+        <v>44016</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="14" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B14" s="134">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B15" s="134">
+        <v>44016</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="16" spans="1:1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="17" spans="1:1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>118</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update read excel for read select sheets, fixed unittest aocs
</commit_message>
<xml_diff>
--- a/organizational/iterations_io.xlsx
+++ b/organizational/iterations_io.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12420" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12420" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 1" sheetId="1" r:id="rId1"/>
@@ -197,9 +197,6 @@
     <t>orbital maneuvers</t>
   </si>
   <si>
-    <t>Nadir</t>
-  </si>
-  <si>
     <t>Driving</t>
   </si>
   <si>
@@ -386,9 +383,6 @@
     <t>Budgets Update</t>
   </si>
   <si>
-    <t>orientation for SA</t>
-  </si>
-  <si>
     <t xml:space="preserve">Comms </t>
   </si>
   <si>
@@ -419,20 +413,26 @@
     <t>Probes</t>
   </si>
   <si>
-    <t>Nominal rates</t>
-  </si>
-  <si>
     <t>Full range</t>
   </si>
   <si>
     <t>Nominal (0.05 - 0.5 deg/s)</t>
+  </si>
+  <si>
+    <t>max excursion 23.5deg</t>
+  </si>
+  <si>
+    <t>Nadir, max excursion 42.4deg</t>
+  </si>
+  <si>
+    <t>Nominal rates 90deg-50min</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -484,8 +484,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -514,6 +521,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="36">
     <border>
@@ -917,13 +929,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1183,6 +1196,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1195,6 +1210,30 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1204,24 +1243,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1249,22 +1270,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="31" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
+    <cellStyle name="Bad" xfId="4" builtinId="27"/>
     <cellStyle name="Explanatory Text" xfId="3" builtinId="53"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
@@ -1583,17 +1599,17 @@
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="23"/>
-      <c r="D3" s="108" t="s">
+      <c r="D3" s="110" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="109"/>
-      <c r="F3" s="109"/>
-      <c r="G3" s="110"/>
+      <c r="E3" s="111"/>
+      <c r="F3" s="111"/>
+      <c r="G3" s="112"/>
       <c r="H3" s="24"/>
-      <c r="J3" s="107" t="s">
+      <c r="J3" s="109" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="107"/>
+      <c r="K3" s="109"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C4" s="25"/>
@@ -1727,12 +1743,12 @@
     <row r="18" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C19" s="23"/>
-      <c r="D19" s="108" t="s">
+      <c r="D19" s="110" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="109"/>
-      <c r="F19" s="109"/>
-      <c r="G19" s="110"/>
+      <c r="E19" s="111"/>
+      <c r="F19" s="111"/>
+      <c r="G19" s="112"/>
       <c r="H19" s="24"/>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
@@ -1892,8 +1908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1901,7 +1917,7 @@
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" style="42" customWidth="1"/>
     <col min="4" max="4" width="19.5703125" style="19" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" style="42" customWidth="1"/>
     <col min="7" max="7" width="24" style="42" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
@@ -1910,62 +1926,63 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="95" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="96" t="s">
-        <v>55</v>
-      </c>
-      <c r="D2" s="111" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="121" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
-      <c r="H2" s="112"/>
-      <c r="I2" s="113"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="122"/>
+      <c r="H2" s="122"/>
+      <c r="I2" s="123"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="97" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" s="126" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="130" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="131"/>
+      <c r="F3" s="130" t="s">
         <v>61</v>
       </c>
-      <c r="E3" s="127"/>
-      <c r="F3" s="126" t="s">
-        <v>62</v>
-      </c>
-      <c r="G3" s="128"/>
+      <c r="G3" s="132"/>
       <c r="H3" s="66"/>
       <c r="I3" s="88"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="98" t="s">
-        <v>93</v>
-      </c>
+      <c r="A4" s="135"/>
       <c r="D4" s="62" t="s">
         <v>45</v>
       </c>
       <c r="E4" s="63" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F4" s="100" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" s="72" t="s">
         <v>59</v>
       </c>
-      <c r="G4" s="72" t="s">
-        <v>60</v>
-      </c>
       <c r="H4" s="64" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I4" s="89" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="129" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="98" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="119" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="49" t="s">
@@ -1974,114 +1991,114 @@
       <c r="E5" s="60" t="s">
         <v>52</v>
       </c>
-      <c r="F5" s="130" t="s">
+      <c r="F5" s="120" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="120" t="s">
-        <v>73</v>
+      <c r="G5" s="124" t="s">
+        <v>72</v>
       </c>
       <c r="H5" s="50"/>
       <c r="I5" s="90" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C6" s="115"/>
+      <c r="C6" s="114"/>
       <c r="D6" s="43" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="F6" s="118"/>
-      <c r="G6" s="121"/>
+        <v>70</v>
+      </c>
+      <c r="F6" s="117"/>
+      <c r="G6" s="125"/>
       <c r="H6" s="44"/>
       <c r="I6" s="36"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C7" s="115"/>
+      <c r="C7" s="114"/>
       <c r="D7" s="43" t="s">
         <v>47</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="F7" s="118"/>
-      <c r="G7" s="121"/>
+      <c r="F7" s="117"/>
+      <c r="G7" s="125"/>
       <c r="H7" s="44"/>
       <c r="I7" s="36"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C8" s="115"/>
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="C8" s="114"/>
       <c r="D8" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="F8" s="118"/>
-      <c r="G8" s="121"/>
+      <c r="E8" s="71" t="s">
+        <v>120</v>
+      </c>
+      <c r="F8" s="117"/>
+      <c r="G8" s="125"/>
       <c r="H8" s="44"/>
       <c r="I8" s="36"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C9" s="116"/>
+      <c r="C9" s="115"/>
       <c r="D9" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="71" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" s="119"/>
-      <c r="G9" s="122"/>
+      <c r="E9" s="136" t="s">
+        <v>121</v>
+      </c>
+      <c r="F9" s="118"/>
+      <c r="G9" s="126"/>
       <c r="H9" s="44"/>
       <c r="I9" s="36"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C10" s="123" t="s">
+      <c r="C10" s="127" t="s">
         <v>48</v>
       </c>
       <c r="D10" s="54" t="s">
         <v>5</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F10" s="103" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G10" s="73" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H10" s="68" t="s">
         <v>5</v>
       </c>
       <c r="I10" s="91" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C11" s="124"/>
+      <c r="C11" s="128"/>
       <c r="D11" s="43" t="s">
         <v>7</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="52" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G11" s="83" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H11" s="44"/>
       <c r="I11" s="36"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="125"/>
+      <c r="C12" s="129"/>
       <c r="D12" s="57" t="s">
         <v>50</v>
       </c>
       <c r="E12" s="86" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F12" s="104"/>
       <c r="G12" s="74"/>
@@ -2089,80 +2106,80 @@
       <c r="I12" s="92"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C13" s="114" t="s">
+      <c r="C13" s="113" t="s">
         <v>49</v>
       </c>
       <c r="D13" s="43" t="s">
         <v>51</v>
       </c>
       <c r="E13" s="81" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F13" s="52" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H13" s="44"/>
       <c r="I13" s="36"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C14" s="115"/>
+      <c r="C14" s="114"/>
       <c r="D14" s="43" t="s">
         <v>7</v>
       </c>
       <c r="E14" s="81" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F14" s="52" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G14" s="83" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H14" s="44" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I14" s="36"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C15" s="115"/>
+      <c r="C15" s="114"/>
       <c r="D15" s="43" t="s">
         <v>47</v>
       </c>
       <c r="E15" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F15" s="52" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G15" s="83" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H15" s="44"/>
       <c r="I15" s="36"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C16" s="116"/>
+      <c r="C16" s="115"/>
       <c r="D16" s="57" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E16" s="105" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F16" s="78" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G16" s="58" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H16" s="58"/>
       <c r="I16" s="92"/>
     </row>
     <row r="17" spans="3:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="C17" s="114" t="s">
-        <v>75</v>
+      <c r="C17" s="113" t="s">
+        <v>74</v>
       </c>
       <c r="D17" s="43" t="s">
         <v>21</v>
@@ -2175,182 +2192,182 @@
 Slew
 Safe</v>
       </c>
-      <c r="F17" s="117" t="s">
-        <v>79</v>
+      <c r="F17" s="116" t="s">
+        <v>78</v>
       </c>
       <c r="G17" s="75"/>
       <c r="H17" s="44"/>
       <c r="I17" s="36" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C18" s="115"/>
+      <c r="C18" s="114"/>
       <c r="D18" s="43" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E18" s="94" t="s">
-        <v>90</v>
-      </c>
-      <c r="F18" s="118"/>
+        <v>89</v>
+      </c>
+      <c r="F18" s="117"/>
       <c r="G18" s="75" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H18" s="44"/>
       <c r="I18" s="36"/>
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C19" s="115"/>
+      <c r="C19" s="114"/>
       <c r="D19" s="43" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E19" s="9"/>
-      <c r="F19" s="118"/>
+      <c r="F19" s="117"/>
       <c r="G19" s="75"/>
       <c r="H19" s="44"/>
       <c r="I19" s="36"/>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C20" s="115"/>
+      <c r="C20" s="114"/>
       <c r="D20" s="43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E20" s="71" t="str">
         <f>G10</f>
         <v>0.1 - 0.5 deg</v>
       </c>
-      <c r="F20" s="118"/>
+      <c r="F20" s="117"/>
       <c r="G20" s="75"/>
       <c r="H20" s="44"/>
       <c r="I20" s="36"/>
     </row>
     <row r="21" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C21" s="116"/>
+      <c r="C21" s="115"/>
       <c r="D21" s="57" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" s="93" t="s">
         <v>77</v>
       </c>
-      <c r="E21" s="93" t="s">
-        <v>78</v>
-      </c>
-      <c r="F21" s="119"/>
+      <c r="F21" s="118"/>
       <c r="G21" s="74"/>
       <c r="H21" s="58"/>
       <c r="I21" s="92"/>
     </row>
     <row r="22" spans="3:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="C22" s="114" t="s">
-        <v>82</v>
+      <c r="C22" s="113" t="s">
+        <v>81</v>
       </c>
       <c r="D22" s="54" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E22" s="6"/>
-      <c r="F22" s="117" t="s">
-        <v>98</v>
+      <c r="F22" s="116" t="s">
+        <v>97</v>
       </c>
       <c r="G22" s="73"/>
       <c r="H22" s="55"/>
       <c r="I22" s="56"/>
     </row>
     <row r="23" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C23" s="115"/>
+      <c r="C23" s="114"/>
       <c r="D23" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E23" s="9"/>
-      <c r="F23" s="118"/>
+      <c r="F23" s="117"/>
       <c r="G23" s="75"/>
       <c r="H23" s="44"/>
       <c r="I23" s="45"/>
     </row>
     <row r="24" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C24" s="116"/>
+      <c r="C24" s="115"/>
       <c r="D24" s="57" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E24" s="99"/>
-      <c r="F24" s="119"/>
+      <c r="F24" s="118"/>
       <c r="G24" s="74"/>
       <c r="H24" s="58"/>
       <c r="I24" s="59"/>
     </row>
     <row r="25" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C25" s="114" t="s">
+      <c r="C25" s="113" t="s">
+        <v>99</v>
+      </c>
+      <c r="D25" s="54" t="s">
         <v>100</v>
       </c>
-      <c r="D25" s="54" t="s">
-        <v>101</v>
-      </c>
       <c r="E25" s="6"/>
-      <c r="F25" s="117" t="s">
-        <v>105</v>
+      <c r="F25" s="116" t="s">
+        <v>104</v>
       </c>
       <c r="G25" s="73"/>
       <c r="H25" s="55"/>
       <c r="I25" s="91"/>
     </row>
     <row r="26" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C26" s="115"/>
+      <c r="C26" s="114"/>
       <c r="D26" s="43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E26" s="9"/>
-      <c r="F26" s="118"/>
+      <c r="F26" s="117"/>
       <c r="G26" s="75"/>
       <c r="H26" s="44"/>
       <c r="I26" s="36"/>
     </row>
     <row r="27" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C27" s="115"/>
+      <c r="C27" s="114"/>
       <c r="D27" s="43" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E27" s="9"/>
-      <c r="F27" s="118" t="s">
-        <v>106</v>
+      <c r="F27" s="117" t="s">
+        <v>105</v>
       </c>
       <c r="G27" s="75"/>
       <c r="H27" s="44"/>
       <c r="I27" s="36"/>
     </row>
     <row r="28" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C28" s="115"/>
+      <c r="C28" s="114"/>
       <c r="D28" s="43" t="s">
         <v>49</v>
       </c>
       <c r="E28" s="9"/>
-      <c r="F28" s="118"/>
+      <c r="F28" s="117"/>
       <c r="G28" s="75"/>
       <c r="H28" s="44"/>
       <c r="I28" s="36"/>
     </row>
     <row r="29" spans="3:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="C29" s="115"/>
+      <c r="C29" s="114"/>
       <c r="D29" s="43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E29" s="9"/>
-      <c r="F29" s="118" t="s">
-        <v>107</v>
+      <c r="F29" s="117" t="s">
+        <v>106</v>
       </c>
       <c r="G29" s="75"/>
       <c r="H29" s="44"/>
       <c r="I29" s="36"/>
     </row>
     <row r="30" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C30" s="116"/>
+      <c r="C30" s="115"/>
       <c r="D30" s="57" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E30" s="11"/>
-      <c r="F30" s="119"/>
+      <c r="F30" s="118"/>
       <c r="G30" s="74"/>
       <c r="H30" s="58"/>
       <c r="I30" s="92"/>
     </row>
     <row r="31" spans="3:9" ht="30" x14ac:dyDescent="0.25">
       <c r="C31" s="61" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D31" s="43"/>
       <c r="E31" s="9"/>
@@ -2721,12 +2738,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C25:C30"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="C5:C9"/>
-    <mergeCell ref="F5:F9"/>
     <mergeCell ref="D2:I2"/>
     <mergeCell ref="C17:C21"/>
     <mergeCell ref="C13:C16"/>
@@ -2737,8 +2748,15 @@
     <mergeCell ref="C10:C12"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:G3"/>
+    <mergeCell ref="C25:C30"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="C5:C9"/>
+    <mergeCell ref="F5:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2746,7 +2764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -2765,78 +2783,78 @@
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="70" t="s">
-        <v>55</v>
-      </c>
-      <c r="D2" s="111" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="121" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
-      <c r="H2" s="112"/>
-      <c r="I2" s="113"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="122"/>
+      <c r="H2" s="122"/>
+      <c r="I2" s="123"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="69" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" s="126" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="130" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="131"/>
+      <c r="F3" s="130" t="s">
         <v>61</v>
       </c>
-      <c r="E3" s="127"/>
-      <c r="F3" s="126" t="s">
-        <v>62</v>
-      </c>
-      <c r="G3" s="128"/>
+      <c r="G3" s="132"/>
       <c r="H3" s="66"/>
       <c r="I3" s="67"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="81" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D4" s="62" t="s">
         <v>45</v>
       </c>
       <c r="E4" s="63" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F4" s="100" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" s="72" t="s">
         <v>59</v>
       </c>
-      <c r="G4" s="72" t="s">
-        <v>60</v>
-      </c>
       <c r="H4" s="64" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I4" s="65" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C5" s="129" t="s">
+      <c r="C5" s="119" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="49" t="s">
         <v>51</v>
       </c>
       <c r="E5" s="80" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F5" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="120" t="s">
-        <v>83</v>
+      <c r="G5" s="124" t="s">
+        <v>82</v>
       </c>
       <c r="H5" s="50"/>
       <c r="I5" s="51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C6" s="115"/>
+      <c r="C6" s="114"/>
       <c r="D6" s="43" t="s">
         <v>7</v>
       </c>
@@ -2844,14 +2862,14 @@
         <v>31</v>
       </c>
       <c r="F6" s="52"/>
-      <c r="G6" s="121"/>
+      <c r="G6" s="125"/>
       <c r="H6" s="44" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I6" s="45"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C7" s="115"/>
+      <c r="C7" s="114"/>
       <c r="D7" s="43" t="s">
         <v>6</v>
       </c>
@@ -2859,12 +2877,12 @@
         <v>32</v>
       </c>
       <c r="F7" s="52"/>
-      <c r="G7" s="121"/>
+      <c r="G7" s="125"/>
       <c r="H7" s="44"/>
       <c r="I7" s="45"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C8" s="116"/>
+      <c r="C8" s="115"/>
       <c r="D8" s="43" t="s">
         <v>50</v>
       </c>
@@ -2872,53 +2890,53 @@
         <v>34</v>
       </c>
       <c r="F8" s="102"/>
-      <c r="G8" s="122"/>
+      <c r="G8" s="126"/>
       <c r="H8" s="44"/>
       <c r="I8" s="45"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C9" s="123" t="s">
+      <c r="C9" s="127" t="s">
         <v>48</v>
       </c>
       <c r="D9" s="54" t="s">
         <v>51</v>
       </c>
       <c r="E9" s="81" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F9" s="103" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G9" s="81" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H9" s="68"/>
       <c r="I9" s="56"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C10" s="124"/>
+      <c r="C10" s="128"/>
       <c r="D10" s="43" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="81" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F10" s="52" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G10" s="83" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H10" s="44"/>
       <c r="I10" s="45"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C11" s="125"/>
+      <c r="C11" s="129"/>
       <c r="D11" s="57" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="82" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F11" s="104"/>
       <c r="G11" s="74"/>
@@ -2926,263 +2944,263 @@
       <c r="I11" s="59"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="114" t="s">
+      <c r="C12" s="113" t="s">
         <v>49</v>
       </c>
       <c r="D12" s="43" t="s">
         <v>51</v>
       </c>
       <c r="E12" s="71" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F12" s="52" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G12" s="84" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H12" s="44"/>
       <c r="I12" s="45"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C13" s="115"/>
+      <c r="C13" s="114"/>
       <c r="D13" s="43"/>
       <c r="E13" s="9"/>
       <c r="F13" s="52" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G13" s="83" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H13" s="44" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I13" s="45"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C14" s="115"/>
+      <c r="C14" s="114"/>
       <c r="D14" s="43" t="s">
         <v>7</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F14" s="52" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G14" s="83" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H14" s="44"/>
       <c r="I14" s="45"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C15" s="116"/>
+      <c r="C15" s="115"/>
       <c r="D15" s="57" t="s">
         <v>47</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F15" s="78" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G15" s="85" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H15" s="58"/>
       <c r="I15" s="59"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C16" s="114" t="s">
-        <v>75</v>
+      <c r="C16" s="113" t="s">
+        <v>74</v>
       </c>
       <c r="D16" s="43" t="s">
         <v>21</v>
       </c>
       <c r="E16" t="s">
-        <v>81</v>
-      </c>
-      <c r="F16" s="117" t="s">
-        <v>79</v>
+        <v>80</v>
+      </c>
+      <c r="F16" s="116" t="s">
+        <v>78</v>
       </c>
       <c r="G16" s="75"/>
       <c r="H16" s="44"/>
-      <c r="I16" s="131" t="s">
-        <v>112</v>
+      <c r="I16" s="133" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C17" s="115"/>
+      <c r="C17" s="114"/>
       <c r="D17" s="43" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E17" s="77" t="s">
-        <v>81</v>
-      </c>
-      <c r="F17" s="118"/>
+        <v>80</v>
+      </c>
+      <c r="F17" s="117"/>
       <c r="G17" s="75" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H17" s="44"/>
-      <c r="I17" s="132"/>
+      <c r="I17" s="134"/>
     </row>
     <row r="18" spans="3:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="C18" s="115"/>
+      <c r="C18" s="114"/>
       <c r="D18" s="43" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E18" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="118"/>
+      <c r="F18" s="117"/>
       <c r="G18" s="75"/>
       <c r="H18" s="44"/>
       <c r="I18" s="28" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="C19" s="114"/>
+      <c r="D19" s="43" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="19" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C19" s="115"/>
-      <c r="D19" s="43" t="s">
-        <v>89</v>
       </c>
       <c r="E19" s="106" t="str">
         <f>G9</f>
         <v>not used</v>
       </c>
-      <c r="F19" s="118"/>
+      <c r="F19" s="117"/>
       <c r="G19" s="75"/>
       <c r="H19" s="44"/>
       <c r="I19" s="28"/>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C20" s="116"/>
+      <c r="C20" s="115"/>
       <c r="D20" s="57" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="F20" s="119"/>
+        <v>109</v>
+      </c>
+      <c r="F20" s="118"/>
       <c r="G20" s="74"/>
       <c r="H20" s="58"/>
       <c r="I20" s="79"/>
     </row>
     <row r="21" spans="3:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="114" t="s">
-        <v>82</v>
+      <c r="C21" s="113" t="s">
+        <v>81</v>
       </c>
       <c r="D21" s="54" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E21" s="6"/>
-      <c r="F21" s="117" t="s">
-        <v>98</v>
+      <c r="F21" s="116" t="s">
+        <v>97</v>
       </c>
       <c r="G21" s="73"/>
       <c r="H21" s="55"/>
       <c r="I21" s="56"/>
     </row>
     <row r="22" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C22" s="115"/>
+      <c r="C22" s="114"/>
       <c r="D22" s="43" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E22" s="9"/>
-      <c r="F22" s="118"/>
+      <c r="F22" s="117"/>
       <c r="G22" s="75"/>
       <c r="H22" s="44"/>
       <c r="I22" s="45"/>
     </row>
     <row r="23" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C23" s="116"/>
+      <c r="C23" s="115"/>
       <c r="D23" s="57" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E23" s="99"/>
-      <c r="F23" s="119"/>
+      <c r="F23" s="118"/>
       <c r="G23" s="74"/>
       <c r="H23" s="58"/>
       <c r="I23" s="59"/>
     </row>
     <row r="24" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C24" s="114" t="s">
+      <c r="C24" s="113" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" s="54" t="s">
         <v>100</v>
       </c>
-      <c r="D24" s="54" t="s">
-        <v>101</v>
-      </c>
       <c r="E24" s="6"/>
-      <c r="F24" s="117" t="s">
-        <v>105</v>
+      <c r="F24" s="116" t="s">
+        <v>104</v>
       </c>
       <c r="G24" s="73"/>
       <c r="H24" s="55"/>
       <c r="I24" s="91"/>
     </row>
     <row r="25" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C25" s="115"/>
+      <c r="C25" s="114"/>
       <c r="D25" s="43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E25" s="9"/>
-      <c r="F25" s="118"/>
+      <c r="F25" s="117"/>
       <c r="G25" s="75"/>
       <c r="H25" s="44"/>
       <c r="I25" s="36"/>
     </row>
     <row r="26" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C26" s="115"/>
+      <c r="C26" s="114"/>
       <c r="D26" s="43" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E26" s="9"/>
-      <c r="F26" s="118" t="s">
-        <v>106</v>
+      <c r="F26" s="117" t="s">
+        <v>105</v>
       </c>
       <c r="G26" s="75"/>
       <c r="H26" s="44"/>
       <c r="I26" s="36"/>
     </row>
     <row r="27" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C27" s="115"/>
+      <c r="C27" s="114"/>
       <c r="D27" s="43" t="s">
         <v>49</v>
       </c>
       <c r="E27" s="9"/>
-      <c r="F27" s="118"/>
+      <c r="F27" s="117"/>
       <c r="G27" s="75"/>
       <c r="H27" s="44"/>
       <c r="I27" s="36"/>
     </row>
     <row r="28" spans="3:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="C28" s="115"/>
+      <c r="C28" s="114"/>
       <c r="D28" s="43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E28" s="9"/>
-      <c r="F28" s="118" t="s">
-        <v>107</v>
+      <c r="F28" s="117" t="s">
+        <v>106</v>
       </c>
       <c r="G28" s="75"/>
       <c r="H28" s="44"/>
       <c r="I28" s="36"/>
     </row>
     <row r="29" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C29" s="116"/>
+      <c r="C29" s="115"/>
       <c r="D29" s="57" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E29" s="11"/>
-      <c r="F29" s="119"/>
+      <c r="F29" s="118"/>
       <c r="G29" s="74"/>
       <c r="H29" s="58"/>
       <c r="I29" s="92"/>
     </row>
     <row r="30" spans="3:9" ht="30" x14ac:dyDescent="0.25">
       <c r="C30" s="61" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D30" s="43"/>
       <c r="E30" s="9"/>
@@ -3553,22 +3571,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="F16:F20"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="C16:C20"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="C24:C29"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="F21:F23"/>
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="D2:I2"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="C5:C8"/>
     <mergeCell ref="G5:G8"/>
+    <mergeCell ref="C24:C29"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="F16:F20"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="C16:C20"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="I16:I17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3588,94 +3606,94 @@
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" style="134" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="108" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B2" s="133" t="s">
+      <c r="B2" s="107" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>116</v>
-      </c>
-      <c r="B6" s="134">
+        <v>114</v>
+      </c>
+      <c r="B6" s="108">
         <v>43986</v>
       </c>
     </row>
     <row r="7" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>100</v>
-      </c>
-      <c r="B7" s="134">
+        <v>99</v>
+      </c>
+      <c r="B7" s="108">
         <v>44016</v>
       </c>
     </row>
     <row r="8" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>116</v>
-      </c>
-      <c r="B14" s="134">
+        <v>114</v>
+      </c>
+      <c r="B14" s="108">
         <v>43986</v>
       </c>
     </row>
     <row r="15" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>100</v>
-      </c>
-      <c r="B15" s="134">
+        <v>99</v>
+      </c>
+      <c r="B15" s="108">
         <v>44016</v>
       </c>
     </row>
     <row r="16" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>